<commit_message>
V01.03.02 / Final Binary Name rule 변경 및 Release note 업데이트
</commit_message>
<xml_diff>
--- a/18. Release Note/CVa_SW_Change_History.xlsx
+++ b/18. Release Note/CVa_SW_Change_History.xlsx
@@ -5,21 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\2.project\CVx\1. doc\18. Release Note\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\PROJECT\Gitlab\HMC\CVa\cva_ptc_heater_doc\18. Release Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11625" tabRatio="722"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="11625" tabRatio="722" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SW" sheetId="12" r:id="rId1"/>
+    <sheet name="Boot" sheetId="13" r:id="rId1"/>
+    <sheet name="App" sheetId="12" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">App!$A$1:$K$18</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>File Name</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -69,35 +73,15 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>CVa-PTC Project Software Change History</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>R7F701695(RENESAS)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>CC-RH</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>HKMC</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>HW Ver</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V0100</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V0101</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>V0102</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -496,10 +480,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>V0103</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">LP2 </t>
     </r>
@@ -743,10 +723,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>V010301</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>077A6CBD</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1005,6 +981,656 @@
   </si>
   <si>
     <t>PTC_Heater_CVa_01.03.01-241030_0x077A6CBD.s19</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>차   종</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>RENESAS / RH850 / R7F701695</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>O E M</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Complier</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC-RH V1.07.00</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ver</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경
+일자</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>변경내용</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Checksum</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Name</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HW VERSION</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>로직
+사양서</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>비 고</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>내용</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boot</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>App</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boot+App</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Option</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.00</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>23.09.04</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Bootloader </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기능</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>구현</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>07697BED</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPBT0 : 0xBA3CFFCF
+OPBT1 : 0xFFFFFDFF
+OPBT2 ~ OPBT7 : 1xFFFFFFFF</t>
+  </si>
+  <si>
+    <t>PTC-Boot-230904.mot</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>23.11.15</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 프로그램 ReCompile 및 Checksum 생성</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>07A6B329</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PTC_Heater_Mva_Boot-01.00-231115-0x07A6B329.mot</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일명 규칙 제정</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKMC CVa Boot Software</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVa(Boot)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dowon</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boot+App</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.00</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.02</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.03</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.03.01</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>V01.03.02</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>25.05.07</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Based : V01.03.01
+2. Alert </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신호</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검출</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">추가
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">   Alert </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신호</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연속</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>누적</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검출</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>고장</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검출</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+   (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>단</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연속</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>검출</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>초</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이내</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>재</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>발생</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>조건</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKMC CVa Software</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC-RH</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>077A378E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0728EAB7</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC-RH V2.06.00
+PTC_Heater_Boot-01.00-231115-0x07A6B329.mot
+PTC_Heater_CVa_01.03.02-250507_0x077A378E.s19
+PTC_Heater_CVa_01.03.02-250507_0x0728EAB7.mot(Boot+App)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1012,7 +1638,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="yy&quot;-&quot;m&quot;-&quot;d;@"/>
+  </numFmts>
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -1043,14 +1673,6 @@
       <sz val="8"/>
       <name val="돋움"/>
       <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="바탕체"/>
-      <family val="1"/>
       <charset val="129"/>
     </font>
     <font>
@@ -1103,6 +1725,45 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1118,7 +1779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1211,6 +1872,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1220,142 +1903,247 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="4"/>
+    <cellStyle name="표준 2" xfId="3"/>
     <cellStyle name="표준_B3 부품원가검토(991115)" xfId="1"/>
     <cellStyle name="표준_SGM18 C69 PCB  제작사양서_v08_060308" xfId="2"/>
-    <cellStyle name="하이퍼링크_KDAC C100 PCB  제작사양서_V03_051228(2)" xfId="3"/>
+    <cellStyle name="표준_이천동CJ0125-2" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1657,13 +2445,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" style="72" customWidth="1"/>
+    <col min="2" max="2" width="7" style="72" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="42" customWidth="1"/>
+    <col min="4" max="4" width="44.77734375" style="42" customWidth="1"/>
+    <col min="5" max="7" width="8.88671875" style="72" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="42" customWidth="1"/>
+    <col min="9" max="9" width="40" style="42" customWidth="1"/>
+    <col min="10" max="11" width="7.77734375" style="42" customWidth="1"/>
+    <col min="12" max="12" width="17.21875" style="42" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="40.5" customHeight="1">
+      <c r="A1" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+    </row>
+    <row r="2" spans="1:12" s="48" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+    </row>
+    <row r="3" spans="1:12" s="48" customFormat="1" ht="24" customHeight="1">
+      <c r="A3" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+    </row>
+    <row r="4" spans="1:12" s="48" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+    </row>
+    <row r="5" spans="1:12" s="48" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A5" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="48" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A6" s="55"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="55"/>
+    </row>
+    <row r="7" spans="1:12" s="48" customFormat="1" ht="40.5">
+      <c r="A7" s="59">
+        <v>1</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="67"/>
+    </row>
+    <row r="8" spans="1:12" s="48" customFormat="1" ht="40.5">
+      <c r="A8" s="59">
+        <v>2</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="65" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="65" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="67" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="48" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A9" s="59"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="69"/>
+    </row>
+    <row r="10" spans="1:12" s="48" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="67"/>
+    </row>
+    <row r="11" spans="1:12" ht="26.25" customHeight="1">
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="67"/>
+    </row>
+    <row r="12" spans="1:12" ht="26.25" customHeight="1">
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="71"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:L3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="3.88671875" style="6" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="6" customWidth="1"/>
@@ -1671,60 +2765,64 @@
     <col min="4" max="4" width="7.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.77734375" style="1" customWidth="1"/>
     <col min="6" max="7" width="10.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="46.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="72" customWidth="1"/>
+    <col min="9" max="9" width="46.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:10" ht="40.5" customHeight="1">
+      <c r="A1" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="5" t="s">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="24" customHeight="1">
+      <c r="A3" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="13" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="40"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="10.9" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1732,211 +2830,262 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="36" t="s">
+      <c r="B5" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="34" t="s">
+      <c r="G5" s="35"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="J5" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="37"/>
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="20" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
+      <c r="H6" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
     </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="51.75" customHeight="1">
       <c r="A7" s="7">
         <v>1</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="25.5">
       <c r="A8" s="10">
         <v>2</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>24</v>
+        <v>31</v>
+      </c>
+      <c r="H8" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="51" customHeight="1">
       <c r="A9" s="10">
         <v>3</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="66" customHeight="1">
       <c r="A10" s="21">
         <v>4</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>30</v>
+      <c r="H10" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="15" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" s="15" customFormat="1" ht="33.75" customHeight="1">
       <c r="A11" s="10">
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="26" t="s">
-        <v>46</v>
+        <v>36</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+    <row r="12" spans="1:10" s="15" customFormat="1" ht="51">
+      <c r="A12" s="10">
+        <v>6</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="J5:J6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>